<commit_message>
Finaliza jornada QH 2015-01-07
</commit_message>
<xml_diff>
--- a/Documentacion/ejemplo acuerdos.xlsx
+++ b/Documentacion/ejemplo acuerdos.xlsx
@@ -373,15 +373,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -414,6 +405,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="41" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,19 +717,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -766,89 +766,89 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="10" t="s">
+    <row r="3" spans="1:11" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="9">
         <v>40179</v>
       </c>
-      <c r="F3" s="10">
-        <v>1</v>
-      </c>
-      <c r="G3" s="10">
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7">
         <v>0</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="7">
         <v>0</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="7">
         <v>0</v>
       </c>
-      <c r="J3" s="10">
-        <v>2</v>
-      </c>
-      <c r="K3" s="10">
+      <c r="J3" s="7">
+        <v>2</v>
+      </c>
+      <c r="K3" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="14" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
-        <v>2</v>
-      </c>
-      <c r="B4" s="14" t="s">
+    <row r="4" spans="1:11" s="11" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="13">
         <v>40544</v>
       </c>
-      <c r="F4" s="14">
-        <v>1</v>
-      </c>
-      <c r="G4" s="14">
+      <c r="F4" s="11">
+        <v>1</v>
+      </c>
+      <c r="G4" s="11">
         <v>0</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="11">
         <v>0</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="11">
         <v>0</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="11">
         <v>0</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="11">
         <v>493</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="8"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -879,70 +879,70 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>1</v>
-      </c>
-      <c r="B12" s="10">
+    <row r="12" spans="1:11" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>1</v>
+      </c>
+      <c r="B12" s="7">
         <v>40</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="7">
         <v>2309109000</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="7">
         <v>0</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="8">
         <v>10</v>
       </c>
-      <c r="I12" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="17" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
-        <v>2</v>
-      </c>
-      <c r="B13" s="17">
+      <c r="I12" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
+        <v>2</v>
+      </c>
+      <c r="B13" s="14">
         <v>0</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="14">
         <v>0</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="15" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="9"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -967,631 +967,631 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>1</v>
-      </c>
-      <c r="B18" s="10" t="s">
+    <row r="18" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>1</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="7">
         <v>0</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="7">
         <v>0</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="10">
-        <v>1</v>
-      </c>
-      <c r="G18" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
-        <v>2</v>
-      </c>
-      <c r="B19" s="10" t="s">
+      <c r="F18" s="7">
+        <v>1</v>
+      </c>
+      <c r="G18" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>2</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="7">
         <v>0</v>
       </c>
-      <c r="D19" s="10">
-        <v>1</v>
-      </c>
-      <c r="E19" s="11" t="s">
+      <c r="D19" s="7">
+        <v>1</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="10">
-        <v>1</v>
-      </c>
-      <c r="G19" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
+      <c r="F19" s="7">
+        <v>1</v>
+      </c>
+      <c r="G19" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
         <v>3</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="10">
         <v>0</v>
       </c>
-      <c r="D20" s="13">
-        <v>1</v>
-      </c>
-      <c r="E20" s="13" t="s">
+      <c r="D20" s="10">
+        <v>1</v>
+      </c>
+      <c r="E20" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="13">
-        <v>1</v>
-      </c>
-      <c r="G20" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="17">
+      <c r="F20" s="10">
+        <v>1</v>
+      </c>
+      <c r="G20" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
         <v>4</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="14">
         <v>0</v>
       </c>
-      <c r="D21" s="17">
-        <v>1</v>
-      </c>
-      <c r="E21" s="18" t="s">
+      <c r="D21" s="14">
+        <v>1</v>
+      </c>
+      <c r="E21" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="17">
-        <v>2</v>
-      </c>
-      <c r="G21" s="17">
+      <c r="F21" s="14">
+        <v>2</v>
+      </c>
+      <c r="G21" s="14">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="6"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="20"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G30" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13">
-        <v>1</v>
-      </c>
-      <c r="B31" s="13">
+    <row r="31" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>1</v>
+      </c>
+      <c r="B31" s="10">
         <v>2010</v>
       </c>
-      <c r="C31" s="13">
+      <c r="C31" s="10">
         <v>2010</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="10">
         <v>2400</v>
       </c>
-      <c r="E31" s="13">
-        <v>2</v>
-      </c>
-      <c r="F31" s="13">
-        <v>1</v>
-      </c>
-      <c r="G31" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13">
-        <v>2</v>
-      </c>
-      <c r="B32" s="13">
+      <c r="E31" s="10">
+        <v>2</v>
+      </c>
+      <c r="F31" s="10">
+        <v>1</v>
+      </c>
+      <c r="G31" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>2</v>
+      </c>
+      <c r="B32" s="10">
         <v>2011</v>
       </c>
-      <c r="C32" s="13">
+      <c r="C32" s="10">
         <v>2011</v>
       </c>
-      <c r="D32" s="13">
+      <c r="D32" s="10">
         <f>D31+48</f>
         <v>2448</v>
       </c>
-      <c r="E32" s="13">
-        <v>2</v>
-      </c>
-      <c r="F32" s="13">
-        <v>1</v>
-      </c>
-      <c r="G32" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="13">
+      <c r="E32" s="10">
+        <v>2</v>
+      </c>
+      <c r="F32" s="10">
+        <v>1</v>
+      </c>
+      <c r="G32" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
         <v>3</v>
       </c>
-      <c r="B33" s="13">
+      <c r="B33" s="10">
         <v>2012</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C33" s="10">
         <v>2012</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D33" s="10">
         <f t="shared" ref="D33:D40" si="0">D32+48</f>
         <v>2496</v>
       </c>
-      <c r="E33" s="13">
-        <v>2</v>
-      </c>
-      <c r="F33" s="13">
-        <v>1</v>
-      </c>
-      <c r="G33" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13">
+      <c r="E33" s="10">
+        <v>2</v>
+      </c>
+      <c r="F33" s="10">
+        <v>1</v>
+      </c>
+      <c r="G33" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
         <v>4</v>
       </c>
-      <c r="B34" s="13">
+      <c r="B34" s="10">
         <v>2013</v>
       </c>
-      <c r="C34" s="13">
+      <c r="C34" s="10">
         <v>2013</v>
       </c>
-      <c r="D34" s="13">
+      <c r="D34" s="10">
         <f t="shared" si="0"/>
         <v>2544</v>
       </c>
-      <c r="E34" s="13">
-        <v>2</v>
-      </c>
-      <c r="F34" s="13">
-        <v>1</v>
-      </c>
-      <c r="G34" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="13">
+      <c r="E34" s="10">
+        <v>2</v>
+      </c>
+      <c r="F34" s="10">
+        <v>1</v>
+      </c>
+      <c r="G34" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
         <v>5</v>
       </c>
-      <c r="B35" s="13">
+      <c r="B35" s="10">
         <v>2014</v>
       </c>
-      <c r="C35" s="13">
+      <c r="C35" s="10">
         <v>2014</v>
       </c>
-      <c r="D35" s="13">
+      <c r="D35" s="10">
         <f t="shared" si="0"/>
         <v>2592</v>
       </c>
-      <c r="E35" s="13">
-        <v>2</v>
-      </c>
-      <c r="F35" s="13">
-        <v>1</v>
-      </c>
-      <c r="G35" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="13">
+      <c r="E35" s="10">
+        <v>2</v>
+      </c>
+      <c r="F35" s="10">
+        <v>1</v>
+      </c>
+      <c r="G35" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
         <v>6</v>
       </c>
-      <c r="B36" s="13">
+      <c r="B36" s="10">
         <v>2015</v>
       </c>
-      <c r="C36" s="13">
+      <c r="C36" s="10">
         <v>2015</v>
       </c>
-      <c r="D36" s="13">
+      <c r="D36" s="10">
         <f t="shared" si="0"/>
         <v>2640</v>
       </c>
-      <c r="E36" s="13">
-        <v>2</v>
-      </c>
-      <c r="F36" s="13">
-        <v>1</v>
-      </c>
-      <c r="G36" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="13">
+      <c r="E36" s="10">
+        <v>2</v>
+      </c>
+      <c r="F36" s="10">
+        <v>1</v>
+      </c>
+      <c r="G36" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
         <v>7</v>
       </c>
-      <c r="B37" s="13">
+      <c r="B37" s="10">
         <v>2016</v>
       </c>
-      <c r="C37" s="13">
+      <c r="C37" s="10">
         <v>2016</v>
       </c>
-      <c r="D37" s="13">
+      <c r="D37" s="10">
         <f t="shared" si="0"/>
         <v>2688</v>
       </c>
-      <c r="E37" s="13">
-        <v>2</v>
-      </c>
-      <c r="F37" s="13">
-        <v>1</v>
-      </c>
-      <c r="G37" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13">
+      <c r="E37" s="10">
+        <v>2</v>
+      </c>
+      <c r="F37" s="10">
+        <v>1</v>
+      </c>
+      <c r="G37" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
         <v>8</v>
       </c>
-      <c r="B38" s="13">
+      <c r="B38" s="10">
         <v>2017</v>
       </c>
-      <c r="C38" s="13">
+      <c r="C38" s="10">
         <v>2017</v>
       </c>
-      <c r="D38" s="13">
+      <c r="D38" s="10">
         <f t="shared" si="0"/>
         <v>2736</v>
       </c>
-      <c r="E38" s="13">
-        <v>2</v>
-      </c>
-      <c r="F38" s="13">
-        <v>1</v>
-      </c>
-      <c r="G38" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="13">
+      <c r="E38" s="10">
+        <v>2</v>
+      </c>
+      <c r="F38" s="10">
+        <v>1</v>
+      </c>
+      <c r="G38" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="10">
         <v>9</v>
       </c>
-      <c r="B39" s="13">
+      <c r="B39" s="10">
         <v>2018</v>
       </c>
-      <c r="C39" s="13">
+      <c r="C39" s="10">
         <v>2018</v>
       </c>
-      <c r="D39" s="13">
+      <c r="D39" s="10">
         <f t="shared" si="0"/>
         <v>2784</v>
       </c>
-      <c r="E39" s="13">
-        <v>2</v>
-      </c>
-      <c r="F39" s="13">
-        <v>1</v>
-      </c>
-      <c r="G39" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="13">
+      <c r="E39" s="10">
+        <v>2</v>
+      </c>
+      <c r="F39" s="10">
+        <v>1</v>
+      </c>
+      <c r="G39" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
         <v>10</v>
       </c>
-      <c r="B40" s="13">
+      <c r="B40" s="10">
         <v>2019</v>
       </c>
-      <c r="C40" s="13">
+      <c r="C40" s="10">
         <v>2019</v>
       </c>
-      <c r="D40" s="13">
+      <c r="D40" s="10">
         <f t="shared" si="0"/>
         <v>2832</v>
       </c>
-      <c r="E40" s="13">
-        <v>2</v>
-      </c>
-      <c r="F40" s="13">
-        <v>1</v>
-      </c>
-      <c r="G40" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="13">
+      <c r="E40" s="10">
+        <v>2</v>
+      </c>
+      <c r="F40" s="10">
+        <v>1</v>
+      </c>
+      <c r="G40" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="10">
         <v>11</v>
       </c>
-      <c r="B41" s="13">
+      <c r="B41" s="10">
         <v>2010</v>
       </c>
-      <c r="C41" s="13">
+      <c r="C41" s="10">
         <v>5000</v>
       </c>
-      <c r="D41" s="13">
+      <c r="D41" s="10">
         <v>1000</v>
       </c>
-      <c r="E41" s="13">
+      <c r="E41" s="10">
         <v>3</v>
       </c>
-      <c r="F41" s="13">
-        <v>1</v>
-      </c>
-      <c r="G41" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="19">
+      <c r="F41" s="10">
+        <v>1</v>
+      </c>
+      <c r="G41" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="16">
         <v>12</v>
       </c>
-      <c r="B42" s="19">
+      <c r="B42" s="16">
         <v>2011</v>
       </c>
-      <c r="C42" s="19">
+      <c r="C42" s="16">
         <v>2011</v>
       </c>
-      <c r="D42" s="20">
+      <c r="D42" s="17">
         <v>3300</v>
       </c>
-      <c r="E42" s="19">
+      <c r="E42" s="16">
         <v>4</v>
       </c>
-      <c r="F42" s="19">
-        <v>2</v>
-      </c>
-      <c r="G42" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="19">
+      <c r="F42" s="16">
+        <v>2</v>
+      </c>
+      <c r="G42" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="16">
         <v>13</v>
       </c>
-      <c r="B43" s="19">
+      <c r="B43" s="16">
         <v>2012</v>
       </c>
-      <c r="C43" s="19">
+      <c r="C43" s="16">
         <v>2012</v>
       </c>
-      <c r="D43" s="20">
+      <c r="D43" s="17">
         <f>ROUNDDOWN(D42*1.1,1)</f>
         <v>3630</v>
       </c>
-      <c r="E43" s="19">
+      <c r="E43" s="16">
         <v>4</v>
       </c>
-      <c r="F43" s="19">
-        <v>2</v>
-      </c>
-      <c r="G43" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="19">
+      <c r="F43" s="16">
+        <v>2</v>
+      </c>
+      <c r="G43" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="16">
         <v>14</v>
       </c>
-      <c r="B44" s="19">
+      <c r="B44" s="16">
         <v>2013</v>
       </c>
-      <c r="C44" s="19">
+      <c r="C44" s="16">
         <v>2013</v>
       </c>
-      <c r="D44" s="20">
+      <c r="D44" s="17">
         <f t="shared" ref="D44:D51" si="1">ROUNDDOWN(D43*1.1,1)</f>
         <v>3993</v>
       </c>
-      <c r="E44" s="19">
+      <c r="E44" s="16">
         <v>4</v>
       </c>
-      <c r="F44" s="19">
-        <v>2</v>
-      </c>
-      <c r="G44" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="19">
+      <c r="F44" s="16">
+        <v>2</v>
+      </c>
+      <c r="G44" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="16">
         <v>15</v>
       </c>
-      <c r="B45" s="19">
+      <c r="B45" s="16">
         <v>2014</v>
       </c>
-      <c r="C45" s="19">
+      <c r="C45" s="16">
         <v>2014</v>
       </c>
-      <c r="D45" s="20">
+      <c r="D45" s="17">
         <f t="shared" si="1"/>
         <v>4392.3</v>
       </c>
-      <c r="E45" s="19">
+      <c r="E45" s="16">
         <v>4</v>
       </c>
-      <c r="F45" s="19">
-        <v>2</v>
-      </c>
-      <c r="G45" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="19">
+      <c r="F45" s="16">
+        <v>2</v>
+      </c>
+      <c r="G45" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="16">
         <v>16</v>
       </c>
-      <c r="B46" s="19">
+      <c r="B46" s="16">
         <v>2015</v>
       </c>
-      <c r="C46" s="19">
+      <c r="C46" s="16">
         <v>2015</v>
       </c>
-      <c r="D46" s="20">
+      <c r="D46" s="17">
         <f t="shared" si="1"/>
         <v>4831.5</v>
       </c>
-      <c r="E46" s="19">
+      <c r="E46" s="16">
         <v>4</v>
       </c>
-      <c r="F46" s="19">
-        <v>2</v>
-      </c>
-      <c r="G46" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="19">
+      <c r="F46" s="16">
+        <v>2</v>
+      </c>
+      <c r="G46" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="16">
         <v>17</v>
       </c>
-      <c r="B47" s="19">
+      <c r="B47" s="16">
         <v>2016</v>
       </c>
-      <c r="C47" s="19">
+      <c r="C47" s="16">
         <v>2016</v>
       </c>
-      <c r="D47" s="20">
+      <c r="D47" s="17">
         <f t="shared" si="1"/>
         <v>5314.6</v>
       </c>
-      <c r="E47" s="19">
+      <c r="E47" s="16">
         <v>4</v>
       </c>
-      <c r="F47" s="19">
-        <v>2</v>
-      </c>
-      <c r="G47" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="19">
+      <c r="F47" s="16">
+        <v>2</v>
+      </c>
+      <c r="G47" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="16">
         <v>18</v>
       </c>
-      <c r="B48" s="19">
+      <c r="B48" s="16">
         <v>2017</v>
       </c>
-      <c r="C48" s="19">
+      <c r="C48" s="16">
         <v>2017</v>
       </c>
-      <c r="D48" s="20">
+      <c r="D48" s="17">
         <f t="shared" si="1"/>
         <v>5846</v>
       </c>
-      <c r="E48" s="19">
+      <c r="E48" s="16">
         <v>4</v>
       </c>
-      <c r="F48" s="19">
-        <v>2</v>
-      </c>
-      <c r="G48" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="19">
+      <c r="F48" s="16">
+        <v>2</v>
+      </c>
+      <c r="G48" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="16">
         <v>19</v>
       </c>
-      <c r="B49" s="19">
+      <c r="B49" s="16">
         <v>2018</v>
       </c>
-      <c r="C49" s="19">
+      <c r="C49" s="16">
         <v>2018</v>
       </c>
-      <c r="D49" s="20">
+      <c r="D49" s="17">
         <f t="shared" si="1"/>
         <v>6430.6</v>
       </c>
-      <c r="E49" s="19">
+      <c r="E49" s="16">
         <v>4</v>
       </c>
-      <c r="F49" s="19">
-        <v>2</v>
-      </c>
-      <c r="G49" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="19">
+      <c r="F49" s="16">
+        <v>2</v>
+      </c>
+      <c r="G49" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="16">
         <v>20</v>
       </c>
-      <c r="B50" s="19">
+      <c r="B50" s="16">
         <v>2019</v>
       </c>
-      <c r="C50" s="19">
+      <c r="C50" s="16">
         <v>2019</v>
       </c>
-      <c r="D50" s="20">
+      <c r="D50" s="17">
         <f t="shared" si="1"/>
         <v>7073.6</v>
       </c>
-      <c r="E50" s="19">
+      <c r="E50" s="16">
         <v>4</v>
       </c>
-      <c r="F50" s="19">
-        <v>2</v>
-      </c>
-      <c r="G50" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="19">
+      <c r="F50" s="16">
+        <v>2</v>
+      </c>
+      <c r="G50" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="16">
         <v>21</v>
       </c>
-      <c r="B51" s="19">
+      <c r="B51" s="16">
         <v>2020</v>
       </c>
-      <c r="C51" s="19">
+      <c r="C51" s="16">
         <v>5000</v>
       </c>
-      <c r="D51" s="20">
+      <c r="D51" s="17">
         <f t="shared" si="1"/>
         <v>7780.9</v>
       </c>
-      <c r="E51" s="19">
+      <c r="E51" s="16">
         <v>4</v>
       </c>
-      <c r="F51" s="19">
-        <v>2</v>
-      </c>
-      <c r="G51" s="19">
+      <c r="F51" s="16">
+        <v>2</v>
+      </c>
+      <c r="G51" s="16">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finaliza jornada QH 2015-01-08
</commit_message>
<xml_diff>
--- a/Documentacion/ejemplo acuerdos.xlsx
+++ b/Documentacion/ejemplo acuerdos.xlsx
@@ -698,7 +698,7 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,6 +930,12 @@
       <c r="G13" s="15" t="s">
         <v>55</v>
       </c>
+      <c r="H13" s="14">
+        <v>10</v>
+      </c>
+      <c r="I13" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Finaliza jornada QH 2015-01-09
</commit_message>
<xml_diff>
--- a/Documentacion/ejemplo acuerdos.xlsx
+++ b/Documentacion/ejemplo acuerdos.xlsx
@@ -124,9 +124,6 @@
     <t xml:space="preserve"> contingente_mcontingente</t>
   </si>
   <si>
-    <t xml:space="preserve"> contingente_contigente_desc</t>
-  </si>
-  <si>
     <t xml:space="preserve"> contingente_acuerdo_det_id</t>
   </si>
   <si>
@@ -207,6 +204,9 @@
   <si>
     <t>crecimiento anual del 10% de las cantidades
 Arancel Intracuota: 0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> contingente_desc</t>
   </si>
 </sst>
 </file>
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,10 +806,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>50</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>13</v>
@@ -873,7 +873,7 @@
         <v>19</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>20</v>
@@ -916,19 +916,19 @@
         <v>0</v>
       </c>
       <c r="C13" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="15" t="s">
         <v>52</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>53</v>
       </c>
       <c r="E13" s="14">
         <v>0</v>
       </c>
       <c r="F13" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="15" t="s">
         <v>54</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>55</v>
       </c>
       <c r="H13" s="14">
         <v>10</v>
@@ -940,7 +940,7 @@
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
@@ -964,13 +964,13 @@
         <v>31</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -978,7 +978,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="7">
         <v>0</v>
@@ -1001,7 +1001,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="7">
         <v>0</v>
@@ -1010,7 +1010,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F19" s="7">
         <v>1</v>
@@ -1024,7 +1024,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="10">
         <v>0</v>
@@ -1033,7 +1033,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F20" s="10">
         <v>1</v>
@@ -1047,7 +1047,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="14">
         <v>0</v>
@@ -1056,7 +1056,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21" s="14">
         <v>2</v>
@@ -1068,7 +1068,7 @@
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" s="19"/>
       <c r="C29" s="19"/>
@@ -1079,25 +1079,25 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="F30" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="G30" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>